<commit_message>
update BOM, found d pad on digikey
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aadarsh/Documents/Coding/HackClub/tars-display/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8ED37D-A32C-C84C-A001-33EA6E4A400F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFF9B48-32DD-7B48-B538-D0A1AA768A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20480" yWindow="620" windowWidth="20480" windowHeight="24980" xr2:uid="{76F3C5F8-0592-3545-9B77-C38043100BE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Component</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Digikey</t>
   </si>
   <si>
-    <t>Sparkfun</t>
-  </si>
-  <si>
     <t>Amazon</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>https://www.digikey.com/en/products/detail/cui-devices/TS04-66-50-BK-160-SMT/15634240</t>
   </si>
   <si>
-    <t>https://www.sparkfun.com/multi-directional-switch-5-position-d-pad-smd.html</t>
-  </si>
-  <si>
     <t>https://www.waveshare.com/0.95inch-rgb-oled-a.htm</t>
   </si>
   <si>
@@ -162,6 +156,9 @@
   </si>
   <si>
     <t>https://cart.jlcpcb.com/quote</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sparkfun-electronics/COM-26850/26266463</t>
   </si>
 </sst>
 </file>
@@ -551,7 +548,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,7 +576,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -597,15 +594,15 @@
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -614,17 +611,17 @@
         <v>5.0599999999999996</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D15" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D12" si="0">B3*C3</f>
         <v>5.0599999999999996</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -645,10 +642,10 @@
         <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -669,10 +666,10 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -693,10 +690,10 @@
         <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -714,13 +711,13 @@
         <v>14.98</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -738,13 +735,13 @@
         <v>11.99</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -762,13 +759,13 @@
         <v>9.99</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -789,10 +786,10 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -810,18 +807,18 @@
         <v>0.95</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -837,10 +834,10 @@
         <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -858,7 +855,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -876,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -894,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -912,7 +909,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update BOM with prices
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aadarsh/Documents/Coding/HackClub/tars-display/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFF9B48-32DD-7B48-B538-D0A1AA768A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB99D16-736F-A143-8CE2-E0A4757D15C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20480" yWindow="620" windowWidth="20480" windowHeight="24980" xr2:uid="{76F3C5F8-0592-3545-9B77-C38043100BE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>Component</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Amazon</t>
   </si>
   <si>
-    <t>Waveshare</t>
-  </si>
-  <si>
     <t>Speaker</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>https://www.digikey.com/en/products/detail/cui-devices/TS04-66-50-BK-160-SMT/15634240</t>
   </si>
   <si>
-    <t>https://www.waveshare.com/0.95inch-rgb-oled-a.htm</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/Micro-Servos-Helicopter-Airplane-Controls/dp/B07MLR1498/</t>
   </si>
   <si>
@@ -159,6 +153,27 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/sparkfun-electronics/COM-26850/26266463</t>
+  </si>
+  <si>
+    <t>In cart?</t>
+  </si>
+  <si>
+    <t>Ordered?</t>
+  </si>
+  <si>
+    <t>Received?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/HiLetgo-Colorful-Display-SSD1331-Resolution/dp/B0711RKXB5/</t>
+  </si>
+  <si>
+    <t>Vender cost with shipping</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -168,7 +183,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -182,6 +197,13 @@
       <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -206,10 +228,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -545,18 +568,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6258E23B-78DB-1D42-9C52-C131A4CAD155}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -576,10 +600,22 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -594,15 +630,21 @@
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="1">
+        <v>6.22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -617,14 +659,20 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
-        <v>29</v>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="1">
+        <v>25.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -642,13 +690,19 @@
         <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="1">
+        <v>25.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -666,13 +720,19 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="1">
+        <v>25.82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -690,13 +750,19 @@
         <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="1">
+        <v>25.82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -714,13 +780,19 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="1">
+        <v>39.71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -728,23 +800,29 @@
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>11.99</v>
+        <v>12.99</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>11.99</v>
+        <v>12.99</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="1">
+        <v>39.71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -762,13 +840,19 @@
         <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="1">
+        <v>39.71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -786,13 +870,19 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="1">
+        <v>25.82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -810,15 +900,21 @@
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="1">
+        <v>25.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -834,13 +930,19 @@
         <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="1">
+        <v>25.82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -855,10 +957,13 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -873,10 +978,13 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -891,10 +999,13 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -909,16 +1020,26 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="D17" s="1">
         <f>SUM(D2:D16)</f>
-        <v>52.99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>53.99</v>
+      </c>
+      <c r="I17" s="1">
+        <f>I2+I3+I7</f>
+        <v>71.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -926,6 +1047,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{CD24DD32-B446-3040-A79F-8A473ED5FE71}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{933264B2-DDB6-1F47-989F-C1485F3D6ECF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update gerbers and readme
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aadarsh/Documents/Coding/HackClub/tars-display/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB99D16-736F-A143-8CE2-E0A4757D15C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2FFA47-2D19-8D47-B837-567AF99470F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20480" yWindow="620" windowWidth="20480" windowHeight="24980" xr2:uid="{76F3C5F8-0592-3545-9B77-C38043100BE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
   <si>
     <t>Component</t>
   </si>
@@ -107,6 +107,9 @@
     <t>Amazon</t>
   </si>
   <si>
+    <t>Waveshare</t>
+  </si>
+  <si>
     <t>Speaker</t>
   </si>
   <si>
@@ -137,6 +140,9 @@
     <t>https://www.digikey.com/en/products/detail/cui-devices/TS04-66-50-BK-160-SMT/15634240</t>
   </si>
   <si>
+    <t>https://www.waveshare.com/0.95inch-rgb-oled-a.htm</t>
+  </si>
+  <si>
     <t>https://www.amazon.com/Micro-Servos-Helicopter-Airplane-Controls/dp/B07MLR1498/</t>
   </si>
   <si>
@@ -167,13 +173,19 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>https://www.amazon.com/HiLetgo-Colorful-Display-SSD1331-Resolution/dp/B0711RKXB5/</t>
-  </si>
-  <si>
     <t>Vender cost with shipping</t>
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Heat inserts</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/HANGLIFE-Heat-Set-Threaded-Printing-Components/dp/B0CS6VZYL8/</t>
   </si>
 </sst>
 </file>
@@ -568,7 +580,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6258E23B-78DB-1D42-9C52-C131A4CAD155}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
@@ -600,19 +612,19 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -630,13 +642,13 @@
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I2" s="1">
         <v>6.22</v>
@@ -644,7 +656,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -660,13 +672,13 @@
         <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I3" s="1">
         <v>25.82</v>
@@ -690,13 +702,13 @@
         <v>21</v>
       </c>
       <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I4" s="1">
         <v>25.82</v>
@@ -720,13 +732,13 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I5" s="1">
         <v>25.82</v>
@@ -750,13 +762,13 @@
         <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I6" s="1">
         <v>25.82</v>
@@ -780,13 +792,13 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I7" s="1">
         <v>39.71</v>
@@ -807,19 +819,16 @@
         <v>12.99</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="1">
-        <v>39.71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -840,13 +849,13 @@
         <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I9" s="1">
         <v>39.71</v>
@@ -870,13 +879,13 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I10" s="1">
         <v>25.82</v>
@@ -900,13 +909,13 @@
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I11" s="1">
         <v>25.82</v>
@@ -914,7 +923,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -930,13 +939,13 @@
         <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I12" s="1">
         <v>25.82</v>
@@ -957,7 +966,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
@@ -978,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
@@ -999,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -1020,27 +1029,54 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I16" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>45</v>
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>8.99</v>
       </c>
       <c r="D17" s="1">
-        <f>SUM(D2:D16)</f>
-        <v>53.99</v>
-      </c>
-      <c r="I17" s="1">
-        <f>I2+I3+I7</f>
+        <f>B17*C17</f>
+        <v>8.99</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1">
+        <f>SUM(D2:D17)</f>
+        <v>62.980000000000004</v>
+      </c>
+      <c r="I18" s="1">
+        <f>I2+I3+I7+I8</f>
         <v>71.75</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>